<commit_message>
Atualização automática de SAO_BORJA.xlsx
</commit_message>
<xml_diff>
--- a/SAO_BORJA.xlsx
+++ b/SAO_BORJA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B5DCA2C5-94A7-4FD0-B2CB-32DD8055975C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{32AE587B-3514-40A7-932D-42C579D6DB08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1207,7 +1207,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{A6B437B3-B20B-4DAD-BFBB-25BEDFB881EF}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{1C5805D1-5A88-4F50-9AD3-44CDA6E50D63}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1237,10 +1237,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8164D89F-40CE-4FF6-8D8E-88A58C0D2674}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2678FEED-F907-4C34-9811-F5B2C189966B}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1278,7 +1278,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7AC4B0B4-71EB-486A-B07A-4C35B28AD634}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6B4D3AE-8719-441B-A129-1A571AD760E4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1341,7 +1341,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0FCAC8E-7D7A-43EE-9F9D-38B209E131EF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A7C62A53-A3F4-41C2-AD7B-2FE70EDB77EC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1360,7 +1360,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C8D672A-D9B9-7385-C110-D0E8D66D5711}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5098D33B-41F0-D53B-79C3-653714CB260E}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1409,7 +1409,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D58F51EB-D8A4-6E0E-96BC-5DAB409A924B}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B7A1CE2D-4B2C-DE66-4046-EB02664B6794}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1428,7 +1428,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF2EBAB9-93C5-CD28-ED04-A8801D2476BD}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0A7CC60-5314-192A-EAC2-89C8EDDFBD19}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1459,7 +1459,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C098EF2-FF9A-F4CB-F38F-C23526C45FF6}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B00E541-7C70-C612-3125-465F3BF6941B}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1490,7 +1490,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C9CEE996-1E51-AA61-59CD-617E6943A5F3}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE853445-3060-1D44-5304-6ABB58B108EF}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1533,7 +1533,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{502FC01A-D4E2-485C-BB2E-5957672B3525}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{14A67F2A-2F32-4833-92B2-4297A3B72876}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1571,7 +1571,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C35F0B20-66FB-4485-8E37-2DB1E4688044}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{16035607-2D56-4B8A-80BE-CAC00544F4EE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1614,7 +1614,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B631BED-9C25-4585-AD5F-89756905D398}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1310847-8134-4243-B309-3C3BA7D31D6B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1927,7 +1927,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BF4EA49-8C90-4833-A8E9-BF4E9AFD181A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{849CD6A7-B627-4614-8416-74E014E2FF11}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>

</xml_diff>